<commit_message>
Cambios en el personaje, creacion del script de movimiento lateral del personaje y salto del personaje.
</commit_message>
<xml_diff>
--- a/Planificacion de tiempo IberianSprint.xlsx
+++ b/Planificacion de tiempo IberianSprint.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92E2109B-6C78-44FF-9063-C20AA11092E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE280DF-4153-4A9E-A263-6E71D443E90E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,6 +35,28 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2534,8 +2556,8 @@
   </sheetPr>
   <dimension ref="A1:BN116"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A98" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="BD98" sqref="BD98"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A47" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="AA56" sqref="AA56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3911,12 +3933,12 @@
       </c>
       <c r="H15" s="51">
         <f ca="1">TODAY()</f>
-        <v>45371</v>
+        <v>45388</v>
       </c>
       <c r="I15" s="13"/>
       <c r="J15" s="13">
         <f t="shared" ca="1" si="6"/>
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="K15" s="24"/>
       <c r="L15" s="24"/>
@@ -3996,7 +4018,7 @@
       </c>
       <c r="H16" s="51">
         <f ca="1">TODAY()</f>
-        <v>45371</v>
+        <v>45388</v>
       </c>
       <c r="I16" s="13"/>
       <c r="J16" s="13"/>
@@ -4522,7 +4544,7 @@
       </c>
       <c r="C23" s="113"/>
       <c r="D23" s="114">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E23" s="115">
         <v>45370</v>
@@ -4536,7 +4558,7 @@
       </c>
       <c r="H23" s="115">
         <f ca="1">TODAY()</f>
-        <v>45371</v>
+        <v>45388</v>
       </c>
       <c r="I23" s="13"/>
       <c r="J23" s="13"/>
@@ -5450,7 +5472,7 @@
       <c r="BM34" s="24"/>
       <c r="BN34" s="24"/>
     </row>
-    <row r="35" spans="1:66" s="3" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:66" s="3" customFormat="1" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="28"/>
       <c r="B35" s="68" t="s">
         <v>45</v>
@@ -5530,7 +5552,7 @@
       <c r="BM35" s="24"/>
       <c r="BN35" s="24"/>
     </row>
-    <row r="36" spans="1:66" s="3" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:66" s="3" customFormat="1" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="28"/>
       <c r="B36" s="68" t="s">
         <v>46</v>
@@ -6826,9 +6848,11 @@
       </c>
       <c r="C53" s="36"/>
       <c r="D53" s="18">
-        <v>0</v>
-      </c>
-      <c r="E53" s="48"/>
+        <v>0.5</v>
+      </c>
+      <c r="E53" s="48">
+        <v>45388</v>
+      </c>
       <c r="F53" s="78">
         <v>2</v>
       </c>
@@ -6836,11 +6860,14 @@
         <f>F53</f>
         <v>2</v>
       </c>
-      <c r="H53" s="48"/>
+      <c r="H53" s="48" cm="1">
+        <f t="array" aca="1" ref="H53" ca="1">hoy</f>
+        <v>45388</v>
+      </c>
       <c r="I53" s="13"/>
-      <c r="J53" s="13" t="str">
-        <f t="shared" si="6"/>
-        <v/>
+      <c r="J53" s="13">
+        <f t="shared" ca="1" si="6"/>
+        <v>1</v>
       </c>
       <c r="K53" s="24"/>
       <c r="L53" s="24"/>
@@ -6906,9 +6933,11 @@
       </c>
       <c r="C54" s="36"/>
       <c r="D54" s="18">
-        <v>0</v>
-      </c>
-      <c r="E54" s="48"/>
+        <v>0.5</v>
+      </c>
+      <c r="E54" s="48">
+        <v>45388</v>
+      </c>
       <c r="F54" s="78">
         <v>0</v>
       </c>
@@ -6916,11 +6945,14 @@
         <f>F54+G53</f>
         <v>2</v>
       </c>
-      <c r="H54" s="48"/>
+      <c r="H54" s="48" cm="1">
+        <f t="array" aca="1" ref="H54" ca="1">hoy</f>
+        <v>45388</v>
+      </c>
       <c r="I54" s="13"/>
-      <c r="J54" s="13" t="str">
-        <f t="shared" si="6"/>
-        <v/>
+      <c r="J54" s="13">
+        <f t="shared" ca="1" si="6"/>
+        <v>1</v>
       </c>
       <c r="K54" s="24"/>
       <c r="L54" s="24"/>
@@ -6993,7 +7025,7 @@
         <v>2</v>
       </c>
       <c r="G55" s="78">
-        <f t="shared" ref="G55:G56" si="15">F55+G54</f>
+        <f>F55+G54</f>
         <v>4</v>
       </c>
       <c r="H55" s="48"/>
@@ -7073,7 +7105,7 @@
         <v>0.5</v>
       </c>
       <c r="G56" s="78">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="G55:G56" si="15">F56+G55</f>
         <v>4.5</v>
       </c>
       <c r="H56" s="48"/>

</xml_diff>